<commit_message>
fix: add pelanggaran modal
</commit_message>
<xml_diff>
--- a/docs/datasets/excel/2425-1.xlsx
+++ b/docs/datasets/excel/2425-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natan\Documents\IFLAB Stuff\data-praktikum-iflab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23457D48-D5E8-497B-8A9A-773AFBB0FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E3803-3936-43E9-B451-216ABA3C740A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="488">
   <si>
     <t>nama_singkat</t>
   </si>
@@ -1356,9 +1356,6 @@
     <t>SE-47-GAMREM</t>
   </si>
   <si>
-    <t>IF-46-GAB PJJ</t>
-  </si>
-  <si>
     <t>DS-46-02</t>
   </si>
   <si>
@@ -1422,9 +1419,6 @@
     <t>IF-46-06</t>
   </si>
   <si>
-    <t>IF-46-02 PJJ</t>
-  </si>
-  <si>
     <t>IF-46-05</t>
   </si>
   <si>
@@ -1507,6 +1501,12 @@
   </si>
   <si>
     <t>GGM</t>
+  </si>
+  <si>
+    <t>IF-46-02PJJ</t>
+  </si>
+  <si>
+    <t>IF-46-GABPJJ</t>
   </si>
 </sst>
 </file>
@@ -1599,9 +1599,7 @@
     <tableColumn id="1" xr3:uid="{21A4836E-464F-4F97-9559-955276C41D49}" name="nama_lengkap"/>
     <tableColumn id="2" xr3:uid="{481E18AF-32E7-4268-BA7E-18ABC65D69EC}" name="nim" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{5AD6B4EF-5D01-443D-9B24-DD656A62BFD5}" name="kode"/>
-    <tableColumn id="4" xr3:uid="{BA910DE9-4FE7-42BF-AB29-8CD75F6813F5}" name="angkatan" dataDxfId="1">
-      <calculatedColumnFormula>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BA910DE9-4FE7-42BF-AB29-8CD75F6813F5}" name="angkatan" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1913,9 +1911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2049,7 +2045,6 @@
         <v>173</v>
       </c>
       <c r="D2">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2064,7 +2059,6 @@
         <v>168</v>
       </c>
       <c r="D3">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2079,7 +2073,6 @@
         <v>259</v>
       </c>
       <c r="D4">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2094,7 +2087,6 @@
         <v>169</v>
       </c>
       <c r="D5">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2109,7 +2101,6 @@
         <v>170</v>
       </c>
       <c r="D6">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -2124,7 +2115,6 @@
         <v>424</v>
       </c>
       <c r="D7">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2139,7 +2129,6 @@
         <v>260</v>
       </c>
       <c r="D8">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2154,7 +2143,6 @@
         <v>360</v>
       </c>
       <c r="D9">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2169,7 +2157,6 @@
         <v>171</v>
       </c>
       <c r="D10">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2184,7 +2171,6 @@
         <v>172</v>
       </c>
       <c r="D11">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2199,7 +2185,6 @@
         <v>274</v>
       </c>
       <c r="D12">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2214,7 +2199,6 @@
         <v>324</v>
       </c>
       <c r="D13">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2229,7 +2213,6 @@
         <v>361</v>
       </c>
       <c r="D14">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2244,7 +2227,6 @@
         <v>349</v>
       </c>
       <c r="D15">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2259,7 +2241,6 @@
         <v>275</v>
       </c>
       <c r="D16">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2274,7 +2255,6 @@
         <v>174</v>
       </c>
       <c r="D17">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -2289,7 +2269,6 @@
         <v>175</v>
       </c>
       <c r="D18">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2304,7 +2283,6 @@
         <v>176</v>
       </c>
       <c r="D19">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2319,7 +2297,6 @@
         <v>362</v>
       </c>
       <c r="D20">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2334,7 +2311,6 @@
         <v>261</v>
       </c>
       <c r="D21">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2349,7 +2325,6 @@
         <v>276</v>
       </c>
       <c r="D22">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2364,7 +2339,6 @@
         <v>299</v>
       </c>
       <c r="D23">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2379,7 +2353,6 @@
         <v>363</v>
       </c>
       <c r="D24">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2394,7 +2367,6 @@
         <v>325</v>
       </c>
       <c r="D25">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2409,7 +2381,6 @@
         <v>177</v>
       </c>
       <c r="D26">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -2424,7 +2395,6 @@
         <v>262</v>
       </c>
       <c r="D27">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2439,7 +2409,6 @@
         <v>263</v>
       </c>
       <c r="D28">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2454,7 +2423,6 @@
         <v>277</v>
       </c>
       <c r="D29">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2469,7 +2437,6 @@
         <v>178</v>
       </c>
       <c r="D30">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2484,7 +2451,6 @@
         <v>364</v>
       </c>
       <c r="D31">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2499,7 +2465,6 @@
         <v>179</v>
       </c>
       <c r="D32">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -2514,7 +2479,6 @@
         <v>278</v>
       </c>
       <c r="D33">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -2529,7 +2493,6 @@
         <v>365</v>
       </c>
       <c r="D34">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2544,7 +2507,6 @@
         <v>180</v>
       </c>
       <c r="D35">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2559,7 +2521,6 @@
         <v>300</v>
       </c>
       <c r="D36">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2574,7 +2535,6 @@
         <v>264</v>
       </c>
       <c r="D37">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2589,7 +2549,6 @@
         <v>181</v>
       </c>
       <c r="D38">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2604,7 +2563,6 @@
         <v>366</v>
       </c>
       <c r="D39">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2619,7 +2577,6 @@
         <v>301</v>
       </c>
       <c r="D40">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2634,7 +2591,6 @@
         <v>265</v>
       </c>
       <c r="D41">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2649,7 +2605,6 @@
         <v>367</v>
       </c>
       <c r="D42">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2664,7 +2619,6 @@
         <v>350</v>
       </c>
       <c r="D43">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2679,7 +2633,6 @@
         <v>182</v>
       </c>
       <c r="D44">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2694,7 +2647,6 @@
         <v>368</v>
       </c>
       <c r="D45">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2709,7 +2661,6 @@
         <v>425</v>
       </c>
       <c r="D46">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2724,7 +2675,6 @@
         <v>351</v>
       </c>
       <c r="D47">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -2739,7 +2689,6 @@
         <v>369</v>
       </c>
       <c r="D48">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2754,7 +2703,6 @@
         <v>183</v>
       </c>
       <c r="D49">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2769,7 +2717,6 @@
         <v>184</v>
       </c>
       <c r="D50">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2784,7 +2731,6 @@
         <v>326</v>
       </c>
       <c r="D51">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2799,7 +2745,6 @@
         <v>302</v>
       </c>
       <c r="D52">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2814,7 +2759,6 @@
         <v>279</v>
       </c>
       <c r="D53">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2829,7 +2773,6 @@
         <v>280</v>
       </c>
       <c r="D54">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2844,7 +2787,6 @@
         <v>370</v>
       </c>
       <c r="D55">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2859,7 +2801,6 @@
         <v>371</v>
       </c>
       <c r="D56">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2874,7 +2815,6 @@
         <v>185</v>
       </c>
       <c r="D57">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2889,7 +2829,6 @@
         <v>327</v>
       </c>
       <c r="D58">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -2904,7 +2843,6 @@
         <v>352</v>
       </c>
       <c r="D59">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2919,7 +2857,6 @@
         <v>186</v>
       </c>
       <c r="D60">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -2934,7 +2871,6 @@
         <v>353</v>
       </c>
       <c r="D61">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2949,7 +2885,6 @@
         <v>187</v>
       </c>
       <c r="D62">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2964,7 +2899,6 @@
         <v>372</v>
       </c>
       <c r="D63">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2979,7 +2913,6 @@
         <v>281</v>
       </c>
       <c r="D64">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -2994,7 +2927,6 @@
         <v>282</v>
       </c>
       <c r="D65">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -3009,7 +2941,6 @@
         <v>328</v>
       </c>
       <c r="D66">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3024,7 +2955,6 @@
         <v>354</v>
       </c>
       <c r="D67">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3039,7 +2969,6 @@
         <v>303</v>
       </c>
       <c r="D68">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3054,7 +2983,6 @@
         <v>188</v>
       </c>
       <c r="D69">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3069,7 +2997,6 @@
         <v>329</v>
       </c>
       <c r="D70">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3084,7 +3011,6 @@
         <v>426</v>
       </c>
       <c r="D71">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3099,7 +3025,6 @@
         <v>283</v>
       </c>
       <c r="D72">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3114,7 +3039,6 @@
         <v>373</v>
       </c>
       <c r="D73">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3129,7 +3053,6 @@
         <v>330</v>
       </c>
       <c r="D74">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3144,7 +3067,6 @@
         <v>266</v>
       </c>
       <c r="D75">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3159,7 +3081,6 @@
         <v>189</v>
       </c>
       <c r="D76">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3174,7 +3095,6 @@
         <v>190</v>
       </c>
       <c r="D77">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3189,7 +3109,6 @@
         <v>191</v>
       </c>
       <c r="D78">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3204,7 +3123,6 @@
         <v>192</v>
       </c>
       <c r="D79">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3219,7 +3137,6 @@
         <v>193</v>
       </c>
       <c r="D80">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3234,7 +3151,6 @@
         <v>355</v>
       </c>
       <c r="D81">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3249,7 +3165,6 @@
         <v>374</v>
       </c>
       <c r="D82">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3264,7 +3179,6 @@
         <v>375</v>
       </c>
       <c r="D83">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3279,7 +3193,6 @@
         <v>304</v>
       </c>
       <c r="D84">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3294,7 +3207,6 @@
         <v>284</v>
       </c>
       <c r="D85">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3309,7 +3221,6 @@
         <v>267</v>
       </c>
       <c r="D86">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3324,7 +3235,6 @@
         <v>268</v>
       </c>
       <c r="D87">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3339,7 +3249,6 @@
         <v>331</v>
       </c>
       <c r="D88">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3354,7 +3263,6 @@
         <v>194</v>
       </c>
       <c r="D89">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3369,7 +3277,6 @@
         <v>195</v>
       </c>
       <c r="D90">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3384,7 +3291,6 @@
         <v>285</v>
       </c>
       <c r="D91">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3399,7 +3305,6 @@
         <v>332</v>
       </c>
       <c r="D92">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3414,7 +3319,6 @@
         <v>376</v>
       </c>
       <c r="D93">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3429,7 +3333,6 @@
         <v>197</v>
       </c>
       <c r="D94">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3444,7 +3347,6 @@
         <v>198</v>
       </c>
       <c r="D95">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3459,7 +3361,6 @@
         <v>269</v>
       </c>
       <c r="D96">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3474,7 +3375,6 @@
         <v>270</v>
       </c>
       <c r="D97">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3489,7 +3389,6 @@
         <v>271</v>
       </c>
       <c r="D98">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3504,7 +3403,6 @@
         <v>377</v>
       </c>
       <c r="D99">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3519,7 +3417,6 @@
         <v>199</v>
       </c>
       <c r="D100">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3534,7 +3431,6 @@
         <v>200</v>
       </c>
       <c r="D101">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3549,7 +3445,6 @@
         <v>201</v>
       </c>
       <c r="D102">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3564,7 +3459,6 @@
         <v>196</v>
       </c>
       <c r="D103">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3579,7 +3473,6 @@
         <v>202</v>
       </c>
       <c r="D104">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3594,7 +3487,6 @@
         <v>356</v>
       </c>
       <c r="D105">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3609,7 +3501,6 @@
         <v>427</v>
       </c>
       <c r="D106">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3624,7 +3515,6 @@
         <v>357</v>
       </c>
       <c r="D107">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3639,7 +3529,6 @@
         <v>272</v>
       </c>
       <c r="D108">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3654,7 +3543,6 @@
         <v>288</v>
       </c>
       <c r="D109">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3669,7 +3557,6 @@
         <v>204</v>
       </c>
       <c r="D110">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3684,7 +3571,6 @@
         <v>305</v>
       </c>
       <c r="D111">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3699,7 +3585,6 @@
         <v>306</v>
       </c>
       <c r="D112">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3714,7 +3599,6 @@
         <v>205</v>
       </c>
       <c r="D113">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3729,7 +3613,6 @@
         <v>358</v>
       </c>
       <c r="D114">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3744,7 +3627,6 @@
         <v>206</v>
       </c>
       <c r="D115">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3759,7 +3641,6 @@
         <v>333</v>
       </c>
       <c r="D116">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3774,7 +3655,6 @@
         <v>307</v>
       </c>
       <c r="D117">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3789,7 +3669,6 @@
         <v>207</v>
       </c>
       <c r="D118">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3804,7 +3683,6 @@
         <v>334</v>
       </c>
       <c r="D119">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3819,7 +3697,6 @@
         <v>273</v>
       </c>
       <c r="D120">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3834,7 +3711,6 @@
         <v>378</v>
       </c>
       <c r="D121">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3849,7 +3725,6 @@
         <v>203</v>
       </c>
       <c r="D122">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3864,7 +3739,6 @@
         <v>335</v>
       </c>
       <c r="D123">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3879,7 +3753,6 @@
         <v>208</v>
       </c>
       <c r="D124">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3894,7 +3767,6 @@
         <v>336</v>
       </c>
       <c r="D125">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3909,7 +3781,6 @@
         <v>308</v>
       </c>
       <c r="D126">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3924,7 +3795,6 @@
         <v>209</v>
       </c>
       <c r="D127">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3939,7 +3809,6 @@
         <v>210</v>
       </c>
       <c r="D128">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>23</v>
       </c>
     </row>
@@ -3954,7 +3823,6 @@
         <v>379</v>
       </c>
       <c r="D129">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -3969,7 +3837,6 @@
         <v>428</v>
       </c>
       <c r="D130" s="3">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -3984,7 +3851,6 @@
         <v>286</v>
       </c>
       <c r="D131">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -3999,7 +3865,6 @@
         <v>380</v>
       </c>
       <c r="D132">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4014,7 +3879,6 @@
         <v>381</v>
       </c>
       <c r="D133">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4029,7 +3893,6 @@
         <v>359</v>
       </c>
       <c r="D134">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4044,7 +3907,6 @@
         <v>382</v>
       </c>
       <c r="D135">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4059,7 +3921,6 @@
         <v>287</v>
       </c>
       <c r="D136">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4074,7 +3935,6 @@
         <v>211</v>
       </c>
       <c r="D137">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4089,7 +3949,6 @@
         <v>212</v>
       </c>
       <c r="D138">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4104,7 +3963,6 @@
         <v>383</v>
       </c>
       <c r="D139">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4119,7 +3977,6 @@
         <v>429</v>
       </c>
       <c r="D140" s="3">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -4134,7 +3991,6 @@
         <v>384</v>
       </c>
       <c r="D141">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4149,7 +4005,6 @@
         <v>213</v>
       </c>
       <c r="D142">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4164,7 +4019,6 @@
         <v>430</v>
       </c>
       <c r="D143" s="3">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4179,7 +4033,6 @@
         <v>214</v>
       </c>
       <c r="D144">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4194,7 +4047,6 @@
         <v>215</v>
       </c>
       <c r="D145">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4209,7 +4061,6 @@
         <v>385</v>
       </c>
       <c r="D146">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>22</v>
       </c>
     </row>
@@ -4224,7 +4075,6 @@
         <v>431</v>
       </c>
       <c r="D147" s="3">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4239,7 +4089,6 @@
         <v>337</v>
       </c>
       <c r="D148">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>20</v>
       </c>
     </row>
@@ -4254,7 +4103,6 @@
         <v>386</v>
       </c>
       <c r="D149">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4269,7 +4117,6 @@
         <v>432</v>
       </c>
       <c r="D150" s="3">
-        <f>INT(MID(Table5[[#This Row],[nim]],IF(LEN(Table5[[#This Row],[nim]])=10,5,6),2))</f>
         <v>21</v>
       </c>
     </row>
@@ -4783,6 +4630,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="6" width="9.88671875" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
@@ -5379,13 +5227,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>437</v>
+        <v>487</v>
       </c>
       <c r="B24" t="s">
         <v>95</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -5503,7 +5354,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B29" t="s">
         <v>38</v>
@@ -5529,7 +5380,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
@@ -5555,7 +5406,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B31" t="s">
         <v>38</v>
@@ -5581,7 +5432,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B32" t="s">
         <v>38</v>
@@ -5599,7 +5450,7 @@
         <v>6</v>
       </c>
       <c r="G32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H32" t="s">
         <v>6</v>
@@ -5607,7 +5458,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
@@ -5633,7 +5484,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B34" t="s">
         <v>38</v>
@@ -5659,7 +5510,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -5685,7 +5536,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B36" t="s">
         <v>58</v>
@@ -5711,7 +5562,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B37" t="s">
         <v>58</v>
@@ -5729,7 +5580,7 @@
         <v>6</v>
       </c>
       <c r="G37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H37" t="s">
         <v>6</v>
@@ -5737,7 +5588,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B38" t="s">
         <v>58</v>
@@ -5763,7 +5614,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B39" t="s">
         <v>58</v>
@@ -5781,7 +5632,7 @@
         <v>6</v>
       </c>
       <c r="G39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H39" t="s">
         <v>6</v>
@@ -5789,7 +5640,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B40" t="s">
         <v>58</v>
@@ -5807,7 +5658,7 @@
         <v>6</v>
       </c>
       <c r="G40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H40" t="s">
         <v>6</v>
@@ -5815,7 +5666,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B41" t="s">
         <v>58</v>
@@ -5833,7 +5684,7 @@
         <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H41" t="s">
         <v>6</v>
@@ -5841,7 +5692,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B42" t="s">
         <v>58</v>
@@ -5867,7 +5718,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B43" t="s">
         <v>58</v>
@@ -5893,7 +5744,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B44" t="s">
         <v>70</v>
@@ -5919,7 +5770,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
@@ -5945,7 +5796,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
@@ -5971,7 +5822,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B47" t="s">
         <v>70</v>
@@ -5994,7 +5845,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B48" t="s">
         <v>80</v>
@@ -6020,7 +5871,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B49" t="s">
         <v>80</v>
@@ -6046,7 +5897,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B50" t="s">
         <v>89</v>
@@ -6064,7 +5915,7 @@
         <v>6</v>
       </c>
       <c r="G50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H50" t="s">
         <v>6</v>
@@ -6072,7 +5923,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>459</v>
+        <v>486</v>
       </c>
       <c r="B51" t="s">
         <v>95</v>
@@ -6098,7 +5949,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B52" t="s">
         <v>95</v>
@@ -6124,7 +5975,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B53" t="s">
         <v>80</v>
@@ -6150,7 +6001,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B54" t="s">
         <v>89</v>
@@ -6176,7 +6027,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B55" t="s">
         <v>95</v>
@@ -6202,7 +6053,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B56" t="s">
         <v>95</v>
@@ -6211,7 +6062,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E56" t="s">
         <v>41</v>
@@ -6280,7 +6131,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
@@ -6329,7 +6180,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B61" t="s">
         <v>80</v>
@@ -6347,7 +6198,7 @@
         <v>6</v>
       </c>
       <c r="G61" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H61" t="s">
         <v>5</v>
@@ -6485,7 +6336,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B67" t="s">
         <v>95</v>
@@ -6508,7 +6359,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B68" t="s">
         <v>38</v>
@@ -6526,7 +6377,7 @@
         <v>6</v>
       </c>
       <c r="G68" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H68" t="s">
         <v>4</v>
@@ -6560,7 +6411,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B70" t="s">
         <v>38</v>
@@ -6586,7 +6437,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B71" t="s">
         <v>38</v>
@@ -6612,7 +6463,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B72" t="s">
         <v>38</v>
@@ -6664,7 +6515,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B74" t="s">
         <v>58</v>
@@ -6690,7 +6541,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B75" t="s">
         <v>58</v>
@@ -6768,7 +6619,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B78" t="s">
         <v>70</v>
@@ -6794,7 +6645,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B79" t="s">
         <v>70</v>
@@ -6812,7 +6663,7 @@
         <v>6</v>
       </c>
       <c r="G79" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H79" t="s">
         <v>4</v>
@@ -6820,7 +6671,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B80" t="s">
         <v>70</v>
@@ -6838,7 +6689,7 @@
         <v>6</v>
       </c>
       <c r="G80" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H80" t="s">
         <v>4</v>
@@ -6890,7 +6741,7 @@
         <v>6</v>
       </c>
       <c r="G82" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H82" t="s">
         <v>4</v>
@@ -6898,7 +6749,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B83" t="s">
         <v>70</v>
@@ -6950,7 +6801,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B85" t="s">
         <v>80</v>
@@ -6976,7 +6827,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B86" t="s">
         <v>80</v>
@@ -7020,7 +6871,7 @@
         <v>3</v>
       </c>
       <c r="G87" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H87" t="s">
         <v>4</v>
@@ -7046,7 +6897,7 @@
         <v>4</v>
       </c>
       <c r="G88" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H88" t="s">
         <v>4</v>
@@ -7132,7 +6983,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B92" t="s">
         <v>95</v>
@@ -7158,7 +7009,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B93" t="s">
         <v>95</v>
@@ -7176,7 +7027,7 @@
         <v>6</v>
       </c>
       <c r="G93" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H93" t="s">
         <v>4</v>
@@ -7184,7 +7035,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B94" t="s">
         <v>38</v>
@@ -7192,6 +7043,9 @@
       <c r="D94" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="E94" t="s">
+        <v>48</v>
+      </c>
       <c r="F94">
         <v>5</v>
       </c>
@@ -7204,7 +7058,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B95" t="s">
         <v>95</v>
@@ -7212,6 +7066,9 @@
       <c r="D95" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="E95" t="s">
+        <v>42</v>
+      </c>
       <c r="F95">
         <v>5</v>
       </c>
@@ -7224,7 +7081,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B96" t="s">
         <v>38</v>
@@ -7250,7 +7107,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B97" t="s">
         <v>38</v>
@@ -7276,7 +7133,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B98" t="s">
         <v>58</v>
@@ -7302,7 +7159,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B99" t="s">
         <v>58</v>
@@ -7328,7 +7185,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B100" t="s">
         <v>58</v>
@@ -7346,7 +7203,7 @@
         <v>2</v>
       </c>
       <c r="G100" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H100" t="s">
         <v>7</v>
@@ -7354,7 +7211,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B101" t="s">
         <v>58</v>
@@ -7372,7 +7229,7 @@
         <v>5</v>
       </c>
       <c r="G101" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H101" t="s">
         <v>7</v>
@@ -7380,7 +7237,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B102" t="s">
         <v>70</v>
@@ -7406,7 +7263,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B103" t="s">
         <v>80</v>
@@ -7432,7 +7289,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B104" t="s">
         <v>80</v>
@@ -7450,7 +7307,7 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H104" t="s">
         <v>7</v>
@@ -7458,7 +7315,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B105" t="s">
         <v>80</v>
@@ -7476,7 +7333,7 @@
         <v>7</v>
       </c>
       <c r="G105" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H105" t="s">
         <v>7</v>
@@ -7484,7 +7341,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B106" t="s">
         <v>95</v>
@@ -7510,7 +7367,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B107" t="s">
         <v>95</v>

</xml_diff>